<commit_message>
Update wrong PN for Green LED
</commit_message>
<xml_diff>
--- a/Hardware Files/FAB/ESP32MiniDrop_BOM.xlsx
+++ b/Hardware Files/FAB/ESP32MiniDrop_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccocz\Designs\ESP32MiniDrop\Hardware Files\FAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{523D8C25-7D6E-4715-AAFD-83A3A9FFCA6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4919461-9C13-4290-8EB1-93199F4E0C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="2565" windowWidth="17805" windowHeight="10785" xr2:uid="{3698AB77-B142-43ED-A78C-6E450EBE364F}"/>
+    <workbookView xWindow="8730" yWindow="495" windowWidth="17805" windowHeight="10785" xr2:uid="{3698AB77-B142-43ED-A78C-6E450EBE364F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>4N25-500E</t>
+  </si>
+  <si>
+    <t>150120GS75000</t>
   </si>
 </sst>
 </file>
@@ -756,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B8A1AA-B891-4D1F-8116-F965D6C275AB}">
   <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +934,7 @@
         <v>36</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>

</xml_diff>